<commit_message>
sofia | bonjean&compartments fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Compartments.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Stability/SSS_Sofia_Compartments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Documents\Проекты\СУХОГРУЗЫ\София\SSS\Stability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Stability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB717785-4994-49E1-97E5-3AEC07F27C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44D3F42-580E-4C76-B456-D24D94EC029A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="53" r:id="rId1"/>
@@ -703,12 +703,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -727,7 +733,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -752,6 +758,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1074,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H20" sqref="A20:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,11 +1621,11 @@
       <c r="F20" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="G20" s="3">
-        <v>66</v>
-      </c>
-      <c r="H20" s="3">
-        <v>89</v>
+      <c r="G20" s="10">
+        <v>68</v>
+      </c>
+      <c r="H20" s="10">
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1664,8 +1673,8 @@
       <c r="F22" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="G22" s="3">
-        <v>26</v>
+      <c r="G22" s="10">
+        <v>28</v>
       </c>
       <c r="H22" s="3">
         <v>68</v>
@@ -1690,8 +1699,8 @@
       <c r="F23" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="G23" s="3">
-        <v>26</v>
+      <c r="G23" s="10">
+        <v>28</v>
       </c>
       <c r="H23" s="3">
         <v>68</v>

</xml_diff>